<commit_message>
Refaktuering af DCD og ER
</commit_message>
<xml_diff>
--- a/Artefakter/ER-Diagram.xlsx
+++ b/Artefakter/ER-Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datamatiker\Git repositories\Ladestander\Artefakter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4649C2A-E634-460A-A5D6-6F56C1531962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA094912-60F1-4CD0-8950-379A3EDB423A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F36F70F8-D511-42D8-99A6-D5599BA297D8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Users</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Bookings</t>
+  </si>
+  <si>
+    <t>Password NvarChar(21)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="B10:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +563,13 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
     <row r="20" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>10</v>
@@ -580,7 +590,9 @@
       <c r="I22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
@@ -593,7 +605,6 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="L11:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ER diagram og sql til forsøg på glemt
</commit_message>
<xml_diff>
--- a/Artefakter/ER-Diagram.xlsx
+++ b/Artefakter/ER-Diagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio 2022\Source\Projekter\Ladestander\Artefakter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datamatiker\Git repositories\Ladestander\Artefakter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6B1D50-3015-4E7D-93F1-491312FBCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC38219-6164-4BB7-A00E-7E4B1B711DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{F36F70F8-D511-42D8-99A6-D5599BA297D8}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="16440" windowHeight="28440" xr2:uid="{F36F70F8-D511-42D8-99A6-D5599BA297D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Users</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Color NVarChar()</t>
+  </si>
+  <si>
+    <t>ForgotPassword</t>
+  </si>
+  <si>
+    <t>Fpid INT (PK)</t>
+  </si>
+  <si>
+    <t>Code NvarChar(8)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,15 +524,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289CD0FF-6716-4BCF-B71D-530B8A2D59C6}">
-  <dimension ref="B10:N30"/>
+  <dimension ref="B3:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -534,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -551,7 +585,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
@@ -563,7 +597,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,7 +609,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
@@ -587,7 +621,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -599,19 +633,19 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -619,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -629,7 +663,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -639,12 +673,12 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -652,7 +686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -660,7 +694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -668,7 +702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>27</v>
       </c>

</xml_diff>